<commit_message>
made configurable (in settings): column numbers and start row for input file
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Setting</t>
   </si>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t xml:space="preserve">Example row for adding fixed role per employee number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col_fname </t>
+  </si>
+  <si>
+    <t xml:space="preserve">col_lname </t>
+  </si>
+  <si>
+    <t xml:space="preserve">col_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">col_date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">col_shifttime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">row_input_start</t>
   </si>
 </sst>
 </file>
@@ -140,7 +158,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,6 +173,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -174,13 +196,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
@@ -253,6 +275,54 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Make file and folder defaults configurable in settings file
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Setting</t>
   </si>
@@ -61,13 +61,13 @@
     <t xml:space="preserve">Example row for adding fixed role per employee number</t>
   </si>
   <si>
-    <t xml:space="preserve">col_fname </t>
-  </si>
-  <si>
-    <t xml:space="preserve">col_lname </t>
-  </si>
-  <si>
-    <t xml:space="preserve">col_id </t>
+    <t xml:space="preserve">col_fname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col_lname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col_id</t>
   </si>
   <si>
     <t xml:space="preserve">col_date </t>
@@ -77,6 +77,24 @@
   </si>
   <si>
     <t xml:space="preserve">row_input_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open_default_folder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_folder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">./Output/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">footer_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./Settings/Footer.xlsx</t>
   </si>
 </sst>
 </file>
@@ -158,24 +176,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,136 +213,266 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.94"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>1234</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>5678</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>1234</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>